<commit_message>
Report Generate Heading Done
</commit_message>
<xml_diff>
--- a/view/site/testing.xlsx
+++ b/view/site/testing.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\lms\Team-IGNIS\view\site\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="21972" windowHeight="5808"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="21975" windowHeight="5805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -52,12 +57,6 @@
   </si>
   <si>
     <t>Tr007</t>
-  </si>
-  <si>
-    <t>Tr008</t>
-  </si>
-  <si>
-    <t>Tr009</t>
   </si>
   <si>
     <t>Tr010</t>
@@ -75,11 +74,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1045B]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +138,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -185,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,9 +224,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,6 +276,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,22 +469,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B18" sqref="B18:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" style="4" customWidth="1"/>
-    <col min="3" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="4" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -461,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -481,7 +525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -501,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -521,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -541,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
@@ -561,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -581,385 +625,163 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>42506</v>
+        <v>42508</v>
       </c>
       <c r="C8" s="2">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
       </c>
       <c r="E8" s="2">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>42507</v>
+        <v>42509</v>
       </c>
       <c r="C9" s="2">
-        <v>8.3000000000000007</v>
+        <v>8.1</v>
       </c>
       <c r="D9" s="2">
         <v>5</v>
       </c>
       <c r="E9" s="2">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>42508</v>
+        <v>42510</v>
       </c>
       <c r="C10" s="2">
-        <v>8.4</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
         <v>5</v>
       </c>
       <c r="E10" s="2">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="3">
-        <v>42509</v>
+        <v>42511</v>
       </c>
       <c r="C11" s="2">
-        <v>8.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D11" s="2">
         <v>5</v>
       </c>
       <c r="E11" s="2">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3">
-        <v>42510</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3">
-        <v>42511</v>
-      </c>
-      <c r="C13" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>7.4</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>42514</v>
-      </c>
-      <c r="C14" s="2">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2">
-        <v>8</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3">
-        <v>42509</v>
-      </c>
-      <c r="C15" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
-        <v>42509</v>
-      </c>
-      <c r="C16" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3">
-        <v>42509</v>
-      </c>
-      <c r="C17" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3">
-        <v>42509</v>
-      </c>
-      <c r="C18" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3">
-        <v>42509</v>
-      </c>
-      <c r="C19" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="3">
-        <v>42509</v>
-      </c>
-      <c r="C20" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="3">
-        <v>42509</v>
-      </c>
-      <c r="C21" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="4">
-        <v>42701</v>
-      </c>
-      <c r="C22" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5.15</v>
-      </c>
-      <c r="E22" s="1">
-        <v>7.55</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="4">
-        <v>42702</v>
-      </c>
-      <c r="C23" s="2">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5.05</v>
-      </c>
-      <c r="E23" s="1">
-        <v>8</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="4">
-        <v>42703</v>
-      </c>
-      <c r="C24" s="2">
-        <v>8.15</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="1">
-        <v>7.45</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="4">
-        <v>42704</v>
-      </c>
-      <c r="C25" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5.25</v>
-      </c>
-      <c r="E25" s="1">
-        <v>7.45</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="4">
-        <v>42705</v>
-      </c>
-      <c r="C26" s="2">
-        <v>8</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5.35</v>
-      </c>
-      <c r="E26" s="1">
-        <v>8.35</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.35</v>
-      </c>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -968,24 +790,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>